<commit_message>
adding purrr and updates to module 1 r 101
</commit_message>
<xml_diff>
--- a/images/ES482_class_schedule.xlsx
+++ b/images/ES482_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marissadyck/Documents/Teaching/ES482/ES482-R-labs.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF41DD76-A7BC-3A44-94CF-FF17595CC900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C916822A-A5FB-4345-BE80-7E638C15B1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12220" yWindow="-20500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,21 +866,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="137">
@@ -1360,7 +1360,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="38" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1443,9 +1443,6 @@
       <c r="E3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>23</v>
-      </c>
       <c r="G3" s="12" t="s">
         <v>1</v>
       </c>
@@ -1470,7 +1467,7 @@
         <v>58</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>11</v>
@@ -1493,7 +1490,9 @@
         <v>3</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="F5"/>
+      <c r="F5" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="G5" s="12" t="s">
         <v>10</v>
       </c>
@@ -1532,14 +1531,14 @@
       <c r="B7" s="11">
         <v>44970</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="27" t="s">
         <v>68</v>
       </c>
       <c r="G7" s="12" t="s">
@@ -1556,10 +1555,10 @@
       <c r="B8" s="15">
         <v>44977</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="17"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
@@ -1580,7 +1579,7 @@
       <c r="E9" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="27" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="12" t="s">
@@ -1606,7 +1605,7 @@
       <c r="E10" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="28" t="s">
         <v>70</v>
       </c>
       <c r="G10" s="12" t="s">
@@ -1623,10 +1622,10 @@
       <c r="B11" s="15">
         <v>44998</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="21"/>
       <c r="F11" s="22"/>
       <c r="G11" s="24"/>
@@ -1737,10 +1736,10 @@
       <c r="B16" s="11">
         <v>45033</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="8"/>
       <c r="F16" s="20" t="s">
         <v>25</v>
@@ -1769,8 +1768,8 @@
     </row>
     <row r="21" spans="2:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="8"/>
       <c r="G21"/>
       <c r="H21"/>

</xml_diff>

<commit_message>
updated sched and assign instructions
</commit_message>
<xml_diff>
--- a/images/ES482_class_schedule.xlsx
+++ b/images/ES482_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marissadyck/Documents/Teaching/ES482/ES482-R-labs.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C916822A-A5FB-4345-BE80-7E638C15B1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E540331-2F83-6341-89D4-E05A1A1AEDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12220" yWindow="-20500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>Day</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Tutorial: Final Reports</t>
   </si>
   <si>
-    <t>Stats Lab 6: Model validation and presentation</t>
-  </si>
-  <si>
     <r>
       <t>Fisher, J. T., &amp; Wilkinson, L. (2005). The response of mammals to forest fire and timber harvest in the North American boreal forest. </t>
     </r>
@@ -425,18 +422,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Stats Lab 2: Data Exploration and Introduction to Modelling</t>
-  </si>
-  <si>
-    <t>Stats Lab 3: Generalized linear modelling I</t>
-  </si>
-  <si>
-    <t>Stats Lab 4: Modelling Your Data I</t>
-  </si>
-  <si>
-    <t>Stats Lab 5: Modelling Your Data II</t>
-  </si>
-  <si>
     <t>Intro to R Part 1</t>
   </si>
   <si>
@@ -480,6 +465,30 @@
   </si>
   <si>
     <t>Stats Assignment 5 DUE, Assign Introductions (35%)</t>
+  </si>
+  <si>
+    <t>Intro to R part 4</t>
+  </si>
+  <si>
+    <t>Intro to R part 5</t>
+  </si>
+  <si>
+    <t>Stats Lab 2: Generalized linear modelling I</t>
+  </si>
+  <si>
+    <t>Stats Lab 3: Modelling Your Data I</t>
+  </si>
+  <si>
+    <t>Stats Lab 4: Modelling Your Data II</t>
+  </si>
+  <si>
+    <t>Stats Lab 5: Model validation and presentation</t>
+  </si>
+  <si>
+    <t>Stats Assignment 6 DUE</t>
+  </si>
+  <si>
+    <t>Intro to R part 4 cont…</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1369,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="38" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1380,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
@@ -1389,7 +1398,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -1415,16 +1424,16 @@
         <v>16</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1441,7 +1450,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>1</v>
@@ -1464,7 +1473,7 @@
         <v>30</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>23</v>
@@ -1473,7 +1482,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1491,7 +1500,7 @@
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>10</v>
@@ -1511,14 +1520,14 @@
         <v>31</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="F6"/>
       <c r="G6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>8</v>
@@ -1532,20 +1541,20 @@
         <v>44970</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D7" s="31"/>
       <c r="E7" s="25" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1574,19 +1583,19 @@
         <v>20</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1600,19 +1609,19 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>68</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1642,16 +1651,19 @@
         <v>27</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>72</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1662,22 +1674,22 @@
         <v>45012</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F13" s="20" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1691,19 +1703,19 @@
         <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1714,19 +1726,19 @@
         <v>45026</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
edits to sem module and show answers for assign 1
</commit_message>
<xml_diff>
--- a/images/ES482_class_schedule.xlsx
+++ b/images/ES482_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marissadyck/Documents/Teaching/ES482/ES482-R-labs.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1CD28A-6A0F-2A4F-BD4E-8C03122096C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E813C06B-196C-6741-98AC-1C7C88A8B50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12220" yWindow="-20500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Day</t>
   </si>
@@ -476,12 +476,6 @@
     <t>Stats Lab 2: Generalized linear modelling I</t>
   </si>
   <si>
-    <t>Stats Lab 3: Modelling Your Data I</t>
-  </si>
-  <si>
-    <t>Stats Lab 4: Modelling Your Data II</t>
-  </si>
-  <si>
     <t>Stats Lab 5: Model validation and presentation</t>
   </si>
   <si>
@@ -489,6 +483,9 @@
   </si>
   <si>
     <t>Intro to R part 4 cont…</t>
+  </si>
+  <si>
+    <t>Stats Lab 3: Modelling Your Data II</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1366,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="38" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1523,7 +1520,7 @@
         <v>66</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6"/>
       <c r="G6" s="12" t="s">
@@ -1611,8 +1608,8 @@
       <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="25" t="s">
-        <v>68</v>
+      <c r="E10" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>65</v>
@@ -1651,13 +1648,13 @@
         <v>27</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>56</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>43</v>
@@ -1677,7 +1674,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>56</v>
@@ -1729,7 +1726,7 @@
         <v>41</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
updated dates and html files
</commit_message>
<xml_diff>
--- a/images/ES482_class_schedule.xlsx
+++ b/images/ES482_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marissadyck/Documents/Teaching/ES482/ES482-R-labs.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038FCE97-F757-0C49-B8C9-5A1DA56A0DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09B48A3-0D43-004D-B4EB-6C4387B1F1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>Week</t>
   </si>
@@ -531,6 +531,9 @@
   <si>
     <t>Final Reports DUE</t>
   </si>
+  <si>
+    <t>Intro to R Part 5</t>
+  </si>
 </sst>
 </file>
 
@@ -1030,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1301,7 +1304,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7">
-        <v>44991</v>
+        <v>44990</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>44</v>
@@ -1327,7 +1330,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="15">
-        <v>44998</v>
+        <v>44997</v>
       </c>
       <c r="C11" s="35" t="s">
         <v>50</v>
@@ -1361,7 +1364,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7">
-        <v>45005</v>
+        <v>45004</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>51</v>
@@ -1385,7 +1388,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7">
-        <v>45012</v>
+        <v>45011</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>56</v>
@@ -1393,8 +1396,8 @@
       <c r="D13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>46</v>
+      <c r="E13" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>58</v>
@@ -1411,7 +1414,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7">
-        <v>45019</v>
+        <v>45018</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>61</v>
@@ -1437,7 +1440,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7">
-        <v>45026</v>
+        <v>45025</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>66</v>
@@ -1461,7 +1464,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7">
-        <v>45033</v>
+        <v>45032</v>
       </c>
       <c r="C16" s="36" t="s">
         <v>69</v>

</xml_diff>